<commit_message>
Changed sheets in perturbation_tests/to_be_reformatted/math_L_curve
</commit_message>
<xml_diff>
--- a/test_files/perturbation_tests/to_be_reformatted/math_L-curve/4-genes_6-edges_artificial-data_Sigmoidal_estimation_fixb-1_fixP-1_no-graph_test1.xlsx
+++ b/test_files/perturbation_tests/to_be_reformatted/math_L-curve/4-genes_6-edges_artificial-data_Sigmoidal_estimation_fixb-1_fixP-1_no-graph_test1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="30">
   <si>
     <t>CIN5</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Strain</t>
-  </si>
-  <si>
-    <t>Deletion</t>
   </si>
   <si>
     <t>wt</t>
@@ -617,10 +614,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -779,10 +776,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -905,7 +902,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="10">
         <v>0.4</v>
@@ -1157,7 +1154,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="9">
         <v>0.4</v>
@@ -1446,7 +1443,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -1568,7 +1565,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1690,10 +1687,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1701,27 +1698,15 @@
     <col min="1" max="1" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1729,7 +1714,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1737,7 +1722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1745,7 +1730,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1753,7 +1738,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1761,7 +1746,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1769,57 +1754,57 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
       <c r="B9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>21</v>
       </c>
       <c r="B14" s="8">
         <v>0.4</v>
@@ -1834,20 +1819,20 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="7">
         <v>3</v>
@@ -1858,80 +1843,69 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="7">
+        <v>21</v>
+      </c>
+      <c r="B17">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
         <v>0.1</v>
       </c>
-      <c r="D18">
+      <c r="D17">
         <v>0.2</v>
       </c>
-      <c r="E18">
+      <c r="E17">
         <v>0.30000000000000004</v>
       </c>
-      <c r="F18">
+      <c r="F17">
         <v>0.4</v>
       </c>
-      <c r="G18">
+      <c r="G17">
         <v>0.5</v>
       </c>
-      <c r="H18">
+      <c r="H17">
         <v>0.60000000000000009</v>
       </c>
-      <c r="I18">
+      <c r="I17">
         <v>0.70000000000000007</v>
       </c>
-      <c r="J18">
+      <c r="J17">
         <v>0.8</v>
       </c>
-      <c r="K18">
+      <c r="K17">
         <v>0.9</v>
       </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N18">
+      <c r="N17">
         <v>1.2000000000000002</v>
       </c>
-      <c r="O18">
+      <c r="O17">
         <v>1.3</v>
       </c>
-      <c r="P18">
+      <c r="P17">
         <v>1.4000000000000001</v>
       </c>
-      <c r="Q18">
+      <c r="Q17">
         <v>1.5</v>
       </c>
-      <c r="R18">
+      <c r="R17">
         <v>1.6</v>
       </c>
-      <c r="S18">
+      <c r="S17">
         <v>1.7000000000000002</v>
       </c>
-      <c r="T18">
+      <c r="T17">
         <v>1.8</v>
       </c>
-      <c r="U18">
+      <c r="U17">
         <v>1.9000000000000001</v>
       </c>
-      <c r="V18">
+      <c r="V17">
         <v>2</v>
       </c>
     </row>
@@ -1955,10 +1929,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>